<commit_message>
Adiciona resolucao exercicios 1.0 e 1.1 bd
</commit_message>
<xml_diff>
--- a/sprint-1-bd/aulas/exemplos_relacionamentos.xlsx
+++ b/sprint-1-bd/aulas/exemplos_relacionamentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.santos\Downloads\SENAI\CT\2021-2S-2D\senai-dev-2s2021-alunos\sprint-1-bd\aulas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B332EBCF-53F9-427D-8CD6-389204F20AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C547B8D-FD2A-4577-9C8A-251065F7775C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{032E1B54-8671-4CF1-BE2B-EB25482D0002}"/>
+    <workbookView xWindow="-23148" yWindow="-36" windowWidth="23256" windowHeight="12576" xr2:uid="{032E1B54-8671-4CF1-BE2B-EB25482D0002}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>Pessoa</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>num_telefone</t>
+  </si>
+  <si>
+    <t>idPessoa (Chave Primária)</t>
   </si>
 </sst>
 </file>
@@ -697,14 +700,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968897E3-740D-404C-B700-F246A0D4F536}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C38" sqref="C37:C38"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
@@ -734,7 +737,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="20"/>

</xml_diff>